<commit_message>
Journal de bord - semaine 3
</commit_message>
<xml_diff>
--- a/Journal de bord - 11.02.19 - 15.02.19.xlsx
+++ b/Journal de bord - 11.02.19 - 15.02.19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinis\Desktop\Journal de bord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinis\Desktop\Journal de bord\IMD-Journal-de-bord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{61B215E2-15F7-4084-9497-7ABBDB3C5B75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC3F53DE-EA3C-4731-9C1F-8562BD89C136}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3705" activeTab="4" xr2:uid="{6FF9F98A-377F-4DA7-9DC3-B2393DBEC313}"/>
   </bookViews>

</xml_diff>